<commit_message>
Data Wrangling: US Crime Rates by Region
</commit_message>
<xml_diff>
--- a/data/Crime_In_US_By_State/Crime_In_US_By_State_1999.xlsx
+++ b/data/Crime_In_US_By_State/Crime_In_US_By_State_1999.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dani/Documents/Datascience Projects/Website/US_Crime_Data/US_Crime_Data_Shiny/data/Crime_In_US_By_State/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A401569-EB56-C74A-822E-B9E82B8E34F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC531F7-BEE2-974A-B6B1-5D621C70AACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="1500" windowWidth="25040" windowHeight="14500" xr2:uid="{D4F35F1E-E65F-204E-ACB6-825373749538}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Murder and nonnegligent manslaugther</t>
-  </si>
-  <si>
     <t>Rape</t>
   </si>
   <si>
@@ -369,6 +366,11 @@
   </si>
   <si>
     <t>Kansas</t>
+  </si>
+  <si>
+    <t>Murder and 
+nonnegligent 
+manslaughter</t>
   </si>
 </sst>
 </file>
@@ -469,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -518,6 +520,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F04C08-8783-2E45-9353-1529D67A7F42}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -872,11 +877,11 @@
       <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>11</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>1</v>
@@ -896,10 +901,10 @@
     </row>
     <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="17">
         <v>1999</v>
@@ -931,10 +936,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="17">
         <v>1999</v>
@@ -966,10 +971,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="17">
         <v>1999</v>
@@ -1001,10 +1006,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="17">
         <v>1999</v>
@@ -1036,10 +1041,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="17">
         <v>1999</v>
@@ -1071,10 +1076,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="17">
         <v>1999</v>
@@ -1106,10 +1111,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="17">
         <v>1999</v>
@@ -1141,10 +1146,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="17">
         <v>1999</v>
@@ -1176,10 +1181,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="17">
         <v>1999</v>
@@ -1211,10 +1216,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="17">
         <v>1999</v>
@@ -1246,10 +1251,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="17">
         <v>1999</v>
@@ -1281,10 +1286,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="17">
         <v>1999</v>
@@ -1316,10 +1321,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="17">
         <v>1999</v>
@@ -1351,10 +1356,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="17">
         <v>1999</v>
@@ -1386,10 +1391,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="17">
         <v>1999</v>
@@ -1421,10 +1426,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="17">
         <v>1999</v>
@@ -1456,10 +1461,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="17">
         <v>1999</v>
@@ -1491,10 +1496,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="17">
         <v>1999</v>
@@ -1526,10 +1531,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="17">
         <v>1999</v>
@@ -1561,10 +1566,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="17">
         <v>1999</v>
@@ -1596,10 +1601,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="17">
         <v>1999</v>
@@ -1631,10 +1636,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="17">
         <v>1999</v>
@@ -1666,10 +1671,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="17">
         <v>1999</v>
@@ -1701,10 +1706,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="17">
         <v>1999</v>
@@ -1736,10 +1741,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="17">
         <v>1999</v>
@@ -1771,10 +1776,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="17">
         <v>1999</v>
@@ -1806,10 +1811,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="17">
         <v>1999</v>
@@ -1841,10 +1846,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" s="17">
         <v>1999</v>
@@ -1876,10 +1881,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="17">
         <v>1999</v>
@@ -1911,10 +1916,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" s="17">
         <v>1999</v>
@@ -1946,10 +1951,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="17">
         <v>1999</v>
@@ -1981,10 +1986,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="17">
         <v>1999</v>
@@ -2016,10 +2021,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="17">
         <v>1999</v>
@@ -2051,10 +2056,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" s="17">
         <v>1999</v>
@@ -2086,10 +2091,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="17">
         <v>1999</v>
@@ -2121,10 +2126,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="17">
         <v>1999</v>
@@ -2156,10 +2161,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="17">
         <v>1999</v>
@@ -2191,10 +2196,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="17">
         <v>1999</v>
@@ -2226,10 +2231,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="17">
         <v>1999</v>
@@ -2261,10 +2266,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="17">
         <v>1999</v>
@@ -2296,10 +2301,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="17">
         <v>1999</v>
@@ -2331,10 +2336,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="17">
         <v>1999</v>
@@ -2366,10 +2371,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="17">
         <v>1999</v>
@@ -2401,10 +2406,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="17">
         <v>1999</v>
@@ -2436,10 +2441,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="17">
         <v>1999</v>
@@ -2471,10 +2476,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" s="17">
         <v>1999</v>
@@ -2506,10 +2511,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="17">
         <v>1999</v>
@@ -2541,10 +2546,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="17">
         <v>1999</v>
@@ -2576,10 +2581,10 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="17">
         <v>1999</v>
@@ -2611,10 +2616,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="17">
         <v>1999</v>

</xml_diff>